<commit_message>
include new fields in medication views
</commit_message>
<xml_diff>
--- a/public/import/CentrosMedicos.xlsx
+++ b/public/import/CentrosMedicos.xlsx
@@ -17,10 +17,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
-    <t>telefono</t>
-  </si>
-  <si>
-    <t>Citas</t>
+    <t>name</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>main_phone</t>
+  </si>
+  <si>
+    <t>phone</t>
   </si>
   <si>
     <t>email</t>
@@ -29,19 +35,13 @@
     <t>web</t>
   </si>
   <si>
-    <t>Observaciones</t>
-  </si>
-  <si>
-    <t>Usuario</t>
-  </si>
-  <si>
-    <t>Password</t>
+    <t>notes</t>
   </si>
   <si>
     <t>Hospital De Vallecas - Hospital Infanta Leonor</t>
   </si>
   <si>
-    <t>Calle Gran Via Del Este, Nº 80 28031, Madrid </t>
+    <t>Calle Gran Via Del Este, Nº 80 28031, Madrid</t>
   </si>
   <si>
     <t>Hospital Del Sureste</t>
@@ -51,10 +51,10 @@
 (Madrid)</t>
   </si>
   <si>
-    <t> 91 839 40 00</t>
-  </si>
-  <si>
-    <t>91 839 45 18 </t>
+    <t>91 839 40 00</t>
+  </si>
+  <si>
+    <t>91 839 45 18</t>
   </si>
   <si>
     <t>citas.sureste@salud.madrid.org</t>
@@ -65,13 +65,13 @@
   </si>
   <si>
     <t>Avenida Del Ventisquero De La Condesa, Nº 42
-28035, Madrid </t>
+28035, Madrid</t>
   </si>
   <si>
     <t>Hospital Moncloa S.A.</t>
   </si>
   <si>
-    <t>Avenida De Valladolid, Nº 83 28008, Madrid </t>
+    <t>Avenida De Valladolid, Nº 83 28008, Madrid</t>
   </si>
   <si>
     <t>Clinica Sear, S.A</t>
@@ -85,7 +85,7 @@
   </si>
   <si>
     <t>Calle De Modesto Lafuente, Nº 14 28010,
-Madrid </t>
+Madrid</t>
   </si>
   <si>
     <t>Hospital
@@ -96,18 +96,18 @@
 Madrid</t>
   </si>
   <si>
-    <t> Hospital
+    <t>Hospital
 Clinico San Carlos</t>
   </si>
   <si>
     <t>Calle Del Profesor Martín Lagos, Nº S/N 28040,
-Madrid </t>
+Madrid</t>
   </si>
   <si>
     <t>Hospital Infantil San Rafael</t>
   </si>
   <si>
-    <t>Calle De Serrano, Nº 199 28016, Madrid </t>
+    <t>Calle De Serrano, Nº 199 28016, Madrid</t>
   </si>
   <si>
     <t>915 64 99 44</t>
@@ -123,14 +123,14 @@
 Universitario La Paz</t>
   </si>
   <si>
-    <t>Paseo De La Castellana, Nº 261 28046, Madrid </t>
+    <t>Paseo De La Castellana, Nº 261 28046, Madrid</t>
   </si>
   <si>
     <t>Hospital
 General Universitario Gregorio Marañon</t>
   </si>
   <si>
-    <t>Calle Del Doctor Esquerdo, Nº 46 28009, Madrid </t>
+    <t>Calle Del Doctor Esquerdo, Nº 46 28009, Madrid</t>
   </si>
   <si>
     <t>Lagos de Rivas. Centro médico</t>
@@ -159,7 +159,7 @@
     <t>Av. Velázquez, 7, 28521 Rivas-Vaciamadrid, Madrid</t>
   </si>
   <si>
-    <t> 916 70 02 57</t>
+    <t>916 70 02 57</t>
   </si>
 </sst>
 </file>
@@ -174,6 +174,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -194,12 +195,14 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -278,10 +281,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -292,25 +295,25 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
       <c r="C1" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="0" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>